<commit_message>
Adicionado Pages e ajustado detalhes
</commit_message>
<xml_diff>
--- a/webAutomation/src/test/resources/DataProvider.xlsx
+++ b/webAutomation/src/test/resources/DataProvider.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DesenvolvimentoUra\webAutomation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automacao\autoMatsionpractice\webAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B12194-3703-4190-B8AA-8A68B32D48F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{18C821E6-0A74-4348-A2AE-CA6FFBF045D0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825"/>
   </bookViews>
   <sheets>
     <sheet name="Teste" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Site</t>
   </si>
@@ -45,16 +44,124 @@
   </si>
   <si>
     <t>http://automationpractice.com</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Faded Short Sleeve T-shirts</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Sobrenome</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Pan</t>
+  </si>
+  <si>
+    <t>Senha</t>
+  </si>
+  <si>
+    <t>Data Nascimento</t>
+  </si>
+  <si>
+    <t>terradonunca</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Movie S/A</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>Rua Capitao Gancho</t>
+  </si>
+  <si>
+    <t>Nome Entrega</t>
+  </si>
+  <si>
+    <t>Sobrenome Entrega</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Codigo Postal</t>
+  </si>
+  <si>
+    <t>Informação adicional</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Endereço Referencia</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>32818</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>407-939-5277</t>
+  </si>
+  <si>
+    <t>Valor Total</t>
+  </si>
+  <si>
+    <t>$18.51</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>peterpan17@movie.com</t>
+  </si>
+  <si>
+    <t>peterpan18@movie.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +188,29 @@
       <b/>
       <sz val="11"/>
       <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,12 +259,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -450,48 +590,268 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFE8BC1-3B9D-4241-970D-C4CDECA82BA8}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="8">
+        <v>19459</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="8">
+        <v>19459</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{F680D6A3-6CAE-42A0-A743-8CA1008752B1}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2" display="peterpan@movie.com"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4" display="peterpan@movie.com"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+Correcao para baixa resolucao +Atualizado planilha com emails não cadastrado
</commit_message>
<xml_diff>
--- a/webAutomation/src/test/resources/DataProvider.xlsx
+++ b/webAutomation/src/test/resources/DataProvider.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automacao\autoMatsionpractice\webAutomation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\autoMatsionpractice\webAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2424F4-C067-480C-97E0-5FB105D8B9C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teste" sheetId="1" r:id="rId1"/>
@@ -19,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -148,16 +144,16 @@
     <t>002</t>
   </si>
   <si>
-    <t>peterpan17@movie.com</t>
-  </si>
-  <si>
-    <t>peterpan18@movie.com</t>
+    <t>peterpan30@movie.com</t>
+  </si>
+  <si>
+    <t>peterpan31@movie.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -590,7 +586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
@@ -846,10 +842,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2" display="peterpan@movie.com"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="D4" r:id="rId4" display="peterpan@movie.com"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" display="peterpan@movie.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D4" r:id="rId4" display="peterpan@movie.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>